<commit_message>
code updates for Current Biology revisions
</commit_message>
<xml_diff>
--- a/virome_abundance_meta_analysis/final_aggregate_tables/bikel_2021_aggregated.xlsx
+++ b/virome_abundance_meta_analysis/final_aggregate_tables/bikel_2021_aggregated.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jglopez/Library/CloudStorage/Dropbox/postdoc_research/lit_review/lit_data/final_aggregate_tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JAL/research/gut_phage_quantification/virome_abundance_meta_analysis/final_aggregate_tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E56B56-A796-144A-9721-110481BD872A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD93E400-C4A5-5B4F-9B8C-BBC9EAC762A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19340" yWindow="5580" windowWidth="15100" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14480" yWindow="4020" windowWidth="15100" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="24">
   <si>
     <t>subject</t>
   </si>
@@ -102,21 +102,6 @@
   </si>
   <si>
     <t>bikel_2021_subject_O-90</t>
-  </si>
-  <si>
-    <t>bikel_2021_subject_OMS-288</t>
-  </si>
-  <si>
-    <t>bikel_2021_subject_OMS-446</t>
-  </si>
-  <si>
-    <t>bikel_2021_subject_OMS-55</t>
-  </si>
-  <si>
-    <t>bikel_2021_subject_OMS-64</t>
-  </si>
-  <si>
-    <t>bikel_2021_subject_OMS-87</t>
   </si>
   <si>
     <t>bikel_2021_subject_NW-10</t>
@@ -189,9 +174,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -229,7 +214,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -335,7 +320,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -477,7 +462,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -488,7 +473,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A16" sqref="A16:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -527,7 +512,7 @@
     </row>
     <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
@@ -807,104 +792,39 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="2">
-        <v>2824597951</v>
-      </c>
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="2">
-        <v>892453630</v>
-      </c>
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="2">
-        <v>854823341</v>
-      </c>
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="2">
-        <v>2051740223</v>
-      </c>
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="2"/>
     </row>
     <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="2">
-        <v>2569533007</v>
-      </c>
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="2"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>

</xml_diff>